<commit_message>
finish use case diagram
</commit_message>
<xml_diff>
--- a/CEPP64‐08 Gantt Chart.xlsx
+++ b/CEPP64‐08 Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A17C4D-E319-4B07-8954-148E6DF7F569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D61C9E40-7547-49A6-9B07-A0E3FD7108ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23880" yWindow="-1155" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1318,11 +1318,11 @@
   </sheetPr>
   <dimension ref="A1:BO59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="H14" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <pane xSplit="6" ySplit="4" topLeftCell="H26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
-      <selection pane="bottomRight" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1916,10 +1916,14 @@
       <c r="D17" s="6">
         <v>2</v>
       </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="E17" s="6">
+        <v>10</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
       <c r="G17" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2539,7 +2543,7 @@
       </c>
       <c r="G58" s="29">
         <f>AVERAGE(G6:G57)</f>
-        <v>0.25750000000000001</v>
+        <v>0.28250000000000003</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -2822,6 +2826,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074C886D97DC2CA43A3C320BBEBDF10BC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2152290d9fcc0329f5ae5ab4ff8c314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="44578a0e-d2a4-4569-89a6-913d1072a7e5" xmlns:ns4="a18590ec-63de-4bfb-82c4-ae33370569f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2a8b9a552455b1f3bf67fd0ee4a1fd6" ns3:_="" ns4:_="">
     <xsd:import namespace="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
@@ -3032,36 +3051,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2DD865-0F33-43A8-B553-74F8F988C566}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E717F02-B222-4674-8658-8EF209B467A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
-    <ds:schemaRef ds:uri="a18590ec-63de-4bfb-82c4-ae33370569f5"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3084,9 +3077,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E717F02-B222-4674-8658-8EF209B467A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2DD865-0F33-43A8-B553-74F8F988C566}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
+    <ds:schemaRef ds:uri="a18590ec-63de-4bfb-82c4-ae33370569f5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update CEPP64‐08 Gantt Chart.xlsx
</commit_message>
<xml_diff>
--- a/CEPP64‐08 Gantt Chart.xlsx
+++ b/CEPP64‐08 Gantt Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2BFE91-0DE5-43D4-B858-7D4BC0ACDDB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7223EA47-D795-4726-BD68-8E8428D40433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1319,10 +1319,10 @@
   <dimension ref="A1:BO59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="H11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
-      <selection pane="bottomRight" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomRight" activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2867,21 +2867,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074C886D97DC2CA43A3C320BBEBDF10BC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2152290d9fcc0329f5ae5ab4ff8c314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="44578a0e-d2a4-4569-89a6-913d1072a7e5" xmlns:ns4="a18590ec-63de-4bfb-82c4-ae33370569f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2a8b9a552455b1f3bf67fd0ee4a1fd6" ns3:_="" ns4:_="">
     <xsd:import namespace="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
@@ -3092,32 +3077,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF287837-3503-445D-B664-B7D777C7A24F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a18590ec-63de-4bfb-82c4-ae33370569f5"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E717F02-B222-4674-8658-8EF209B467A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2DD865-0F33-43A8-B553-74F8F988C566}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3134,4 +3109,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E717F02-B222-4674-8658-8EF209B467A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF287837-3503-445D-B664-B7D777C7A24F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a18590ec-63de-4bfb-82c4-ae33370569f5"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add Progress Report 3, Gantt Chart 3, Report 1
</commit_message>
<xml_diff>
--- a/CEPP64‐08 Gantt Chart.xlsx
+++ b/CEPP64‐08 Gantt Chart.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D7DB76-A44D-4113-8766-4729D6953748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA4BEA2-8607-4CDA-9270-F1BAC34A4EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -1319,7 +1319,7 @@
   <dimension ref="A1:BO59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="66" zoomScaleNormal="66" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="H44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
       <selection pane="bottomRight" activeCell="M61" sqref="M61"/>
@@ -2899,6 +2899,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074C886D97DC2CA43A3C320BBEBDF10BC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2152290d9fcc0329f5ae5ab4ff8c314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="44578a0e-d2a4-4569-89a6-913d1072a7e5" xmlns:ns4="a18590ec-63de-4bfb-82c4-ae33370569f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2a8b9a552455b1f3bf67fd0ee4a1fd6" ns3:_="" ns4:_="">
     <xsd:import namespace="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
@@ -3109,22 +3124,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF287837-3503-445D-B664-B7D777C7A24F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a18590ec-63de-4bfb-82c4-ae33370569f5"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E717F02-B222-4674-8658-8EF209B467A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2DD865-0F33-43A8-B553-74F8F988C566}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3141,29 +3166,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E717F02-B222-4674-8658-8EF209B467A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF287837-3503-445D-B664-B7D777C7A24F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a18590ec-63de-4bfb-82c4-ae33370569f5"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update review paper & progress report 4
</commit_message>
<xml_diff>
--- a/CEPP64‐08 Gantt Chart.xlsx
+++ b/CEPP64‐08 Gantt Chart.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25128"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA4BEA2-8607-4CDA-9270-F1BAC34A4EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160104AC-74AB-4CF1-9346-7B64BD6FED80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1319,7 +1319,7 @@
   <dimension ref="A1:BO59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="66" zoomScaleNormal="66" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="H10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
       <selection pane="bottomRight" activeCell="M61" sqref="M61"/>
@@ -2899,21 +2899,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074C886D97DC2CA43A3C320BBEBDF10BC" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2152290d9fcc0329f5ae5ab4ff8c314">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="44578a0e-d2a4-4569-89a6-913d1072a7e5" xmlns:ns4="a18590ec-63de-4bfb-82c4-ae33370569f5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f2a8b9a552455b1f3bf67fd0ee4a1fd6" ns3:_="" ns4:_="">
     <xsd:import namespace="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
@@ -3124,32 +3109,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF287837-3503-445D-B664-B7D777C7A24F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a18590ec-63de-4bfb-82c4-ae33370569f5"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E717F02-B222-4674-8658-8EF209B467A1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB2DD865-0F33-43A8-B553-74F8F988C566}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3166,4 +3141,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E717F02-B222-4674-8658-8EF209B467A1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF287837-3503-445D-B664-B7D777C7A24F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="44578a0e-d2a4-4569-89a6-913d1072a7e5"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a18590ec-63de-4bfb-82c4-ae33370569f5"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>